<commit_message>
appending to existing excel
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,8 +25,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
-      <color rgb="00000000"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,7 +61,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -423,27 +424,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C1:O11"/>
+  <dimension ref="C1:O31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="12" customWidth="1" min="14" max="14"/>
-    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="3" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -539,7 +528,7 @@
       <c r="I2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="n"/>
       <c r="K2" s="2" t="n">
         <v>120</v>
       </c>
@@ -550,7 +539,7 @@
         <v>40.869</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>2447.570059291716</v>
+        <v>2447.57</v>
       </c>
       <c r="O2" s="2" t="n">
         <v>3</v>
@@ -582,7 +571,7 @@
       <c r="I3" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="2" t="inlineStr"/>
+      <c r="J3" s="2" t="n"/>
       <c r="K3" s="2" t="n">
         <v>120</v>
       </c>
@@ -593,7 +582,7 @@
         <v>39.839</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>2371.116599765962</v>
+        <v>2371.12</v>
       </c>
       <c r="O3" s="2" t="n">
         <v>3</v>
@@ -625,7 +614,7 @@
       <c r="I4" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="2" t="inlineStr"/>
+      <c r="J4" s="2" t="n"/>
       <c r="K4" s="2" t="n">
         <v>120</v>
       </c>
@@ -636,7 +625,7 @@
         <v>38.164</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>2168.434390383533</v>
+        <v>2168.43</v>
       </c>
       <c r="O4" s="2" t="n">
         <v>3</v>
@@ -668,7 +657,7 @@
       <c r="I5" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="n"/>
       <c r="K5" s="2" t="n">
         <v>120</v>
       </c>
@@ -679,7 +668,7 @@
         <v>41.211</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>2538.741440576568</v>
+        <v>2538.74</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>3</v>
@@ -711,7 +700,7 @@
       <c r="I6" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J6" s="2" t="inlineStr"/>
+      <c r="J6" s="2" t="n"/>
       <c r="K6" s="2" t="n">
         <v>120</v>
       </c>
@@ -722,7 +711,7 @@
         <v>38.672</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>2192.560188334923</v>
+        <v>2192.56</v>
       </c>
       <c r="O6" s="2" t="n">
         <v>3</v>
@@ -754,7 +743,7 @@
       <c r="I7" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="n"/>
       <c r="K7" s="2" t="n">
         <v>120</v>
       </c>
@@ -765,7 +754,7 @@
         <v>38.984</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>2195.920234775273</v>
+        <v>2195.92</v>
       </c>
       <c r="O7" s="2" t="n">
         <v>3</v>
@@ -797,7 +786,7 @@
       <c r="I8" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J8" s="2" t="inlineStr"/>
+      <c r="J8" s="2" t="n"/>
       <c r="K8" s="2" t="n">
         <v>120</v>
       </c>
@@ -808,7 +797,7 @@
         <v>37.852</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>2053.196147425473</v>
+        <v>2053.2</v>
       </c>
       <c r="O8" s="2" t="n">
         <v>3</v>
@@ -840,7 +829,7 @@
       <c r="I9" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J9" s="2" t="inlineStr"/>
+      <c r="J9" s="2" t="n"/>
       <c r="K9" s="2" t="n">
         <v>120</v>
       </c>
@@ -851,7 +840,7 @@
         <v>36.133</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>2261.449163989731</v>
+        <v>2261.45</v>
       </c>
       <c r="O9" s="2" t="n">
         <v>4</v>
@@ -883,7 +872,7 @@
       <c r="I10" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J10" s="2" t="inlineStr"/>
+      <c r="J10" s="2" t="n"/>
       <c r="K10" s="2" t="n">
         <v>120</v>
       </c>
@@ -894,7 +883,7 @@
         <v>38.633</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>2147.62709130965</v>
+        <v>2147.63</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>3</v>
@@ -926,7 +915,7 @@
       <c r="I11" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="J11" s="2" t="inlineStr"/>
+      <c r="J11" s="2" t="n"/>
       <c r="K11" s="2" t="n">
         <v>110</v>
       </c>
@@ -937,9 +926,869 @@
         <v>39.414</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>2350.650760397597</v>
+        <v>2350.65</v>
       </c>
       <c r="O11" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>11:01:05:3</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>83.983</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J12" s="2" t="n"/>
+      <c r="K12" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>19.063</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>40.869</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>2447.57</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>11:40:46:8</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>84.02500000000001</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0.215</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J13" s="2" t="n"/>
+      <c r="K13" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>18.945</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>39.839</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>2371.12</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>14:34:43:9</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>83.97499999999999</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>1.474</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J14" s="2" t="n"/>
+      <c r="K14" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>18.086</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>38.164</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>2168.43</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>15:09:50:5</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>84.16500000000001</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0.911</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J15" s="2" t="n"/>
+      <c r="K15" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>19.609</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>41.211</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>2538.74</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>21:51:34:5</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>83.878</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>2.328</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J16" s="2" t="n"/>
+      <c r="K16" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>18.047</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>38.672</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>2192.56</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>22:15:43:5</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>83.869</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>3.013</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J17" s="2" t="n"/>
+      <c r="K17" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>17.93</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>38.984</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>2195.92</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>30.04.2012</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>6:16:24:3</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>83.816</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>1.807</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J18" s="2" t="n"/>
+      <c r="K18" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>17.266</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>37.852</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>2053.2</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>30.04.2012</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>8:25:53:3</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>84.01900000000001</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>1.495</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J19" s="2" t="n"/>
+      <c r="K19" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>19.922</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>36.133</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>2261.45</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>1.05.2012</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>1:34:45:7</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>83.959</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>3.238</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J20" s="2" t="n"/>
+      <c r="K20" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>17.695</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>38.633</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>2147.63</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>1.05.2012</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>4:45:31:3</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>84.044</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>-0.148</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J21" s="2" t="n"/>
+      <c r="K21" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>18.984</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>39.414</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>2350.65</v>
+      </c>
+      <c r="O21" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>11:01:05:3</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>84.004</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J22" s="2" t="inlineStr"/>
+      <c r="K22" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>19.297</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>41.016</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>2486.53</v>
+      </c>
+      <c r="O22" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>11:40:46:8</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>84.045</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>-0.08599999999999999</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J23" s="2" t="inlineStr"/>
+      <c r="K23" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>19.18</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>40.093</v>
+      </c>
+      <c r="N23" s="2" t="n">
+        <v>2415.83</v>
+      </c>
+      <c r="O23" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>14:34:43:9</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>83.997</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>1.181</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J24" s="2" t="inlineStr"/>
+      <c r="K24" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>18.281</v>
+      </c>
+      <c r="M24" s="2" t="n">
+        <v>38.359</v>
+      </c>
+      <c r="N24" s="2" t="n">
+        <v>2203.01</v>
+      </c>
+      <c r="O24" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>15:09:50:6</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>84.18600000000001</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>0.614</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J25" s="2" t="inlineStr"/>
+      <c r="K25" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>19.766</v>
+      </c>
+      <c r="M25" s="2" t="n">
+        <v>41.26</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>2562.11</v>
+      </c>
+      <c r="O25" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>21:51:34:5</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>83.90000000000001</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>2.022</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J26" s="2" t="inlineStr"/>
+      <c r="K26" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>18.242</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <v>38.711</v>
+      </c>
+      <c r="N26" s="2" t="n">
+        <v>2218.49</v>
+      </c>
+      <c r="O26" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>29.04.2012</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>22:15:43:5</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>83.89</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>2.716</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J27" s="2" t="inlineStr"/>
+      <c r="K27" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>18.086</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>39.063</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>2219.51</v>
+      </c>
+      <c r="O27" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>30.04.2012</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>6:16:24:3</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>83.837</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>1.508</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J28" s="2" t="inlineStr"/>
+      <c r="K28" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>17.461</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>38.008</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>2084.94</v>
+      </c>
+      <c r="O28" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>30.04.2012</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>8:25:53:3</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>84.039</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>1.213</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J29" s="2" t="inlineStr"/>
+      <c r="K29" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>20.098</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>36.25</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>2288.82</v>
+      </c>
+      <c r="O29" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>1.05.2012</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>1:34:45:7</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>83.979</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>2.945</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J30" s="2" t="inlineStr"/>
+      <c r="K30" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>17.734</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>38.594</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>2150.19</v>
+      </c>
+      <c r="O30" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>1.05.2012</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>4:45:31:2</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>84.063</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>-0.497</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J31" s="2" t="inlineStr"/>
+      <c r="K31" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>19.18</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>39.688</v>
+      </c>
+      <c r="N31" s="2" t="n">
+        <v>2391.43</v>
+      </c>
+      <c r="O31" s="2" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>